<commit_message>
a few css changes, added failing google test, added type to data labels, updated license
</commit_message>
<xml_diff>
--- a/templates/standard label.googlesearch.xlsx
+++ b/templates/standard label.googlesearch.xlsx
@@ -13,7 +13,6 @@
     <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -604,9 +603,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt numFmtId="165" formatCode="h:mm;@"/>
-    <numFmt numFmtId="171" formatCode="[$-409]d\-mmm\-yyyy;@"/>
-    <numFmt numFmtId="172" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="h:mm;@"/>
+    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -688,10 +687,10 @@
     </xf>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Heading" xfId="1"/>
@@ -993,8 +992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
-      <selection activeCell="AE1" sqref="AE1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2215,11 +2214,11 @@
       </c>
       <c r="D25" s="4">
         <f ca="1">NOW()</f>
-        <v>41116.644354976852</v>
+        <v>41123.439263194443</v>
       </c>
       <c r="E25" s="5">
         <f ca="1">D25-C25</f>
-        <v>41116.33810497685</v>
+        <v>41123.133013194441</v>
       </c>
       <c r="F25" s="5">
         <v>41115.077201041662</v>
@@ -2251,7 +2250,7 @@
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.1"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="27.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="4.85546875" customWidth="1"/>
@@ -2315,7 +2314,7 @@
       </c>
       <c r="Q1" s="1"/>
     </row>
-    <row r="2" spans="1:17" ht="15">
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -2344,7 +2343,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15">
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -2373,7 +2372,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15">
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -2405,7 +2404,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15">
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -2434,7 +2433,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15">
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -2466,7 +2465,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15">
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -2495,7 +2494,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15">
+    <row r="8" spans="1:17">
       <c r="A8" t="s">
         <v>41</v>
       </c>
@@ -2524,7 +2523,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15">
+    <row r="9" spans="1:17">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -2553,7 +2552,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15">
+    <row r="10" spans="1:17">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -2582,7 +2581,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="15">
+    <row r="11" spans="1:17">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -2611,7 +2610,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="15">
+    <row r="12" spans="1:17">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -2640,7 +2639,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="15">
+    <row r="13" spans="1:17">
       <c r="C13" t="s">
         <v>0</v>
       </c>
@@ -2666,7 +2665,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="15">
+    <row r="14" spans="1:17">
       <c r="A14" t="s">
         <v>57</v>
       </c>
@@ -2698,7 +2697,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="15">
+    <row r="15" spans="1:17">
       <c r="A15" t="s">
         <v>61</v>
       </c>
@@ -2730,7 +2729,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="15">
+    <row r="16" spans="1:17">
       <c r="A16" t="s">
         <v>67</v>
       </c>
@@ -2759,7 +2758,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="15">
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
         <v>70</v>
       </c>
@@ -2788,7 +2787,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="15">
+    <row r="19" spans="1:13">
       <c r="M19" t="s">
         <v>99</v>
       </c>
@@ -2801,21 +2800,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="E1:E23"/>
+  <dimension ref="E7:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.1"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1024" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="5:5" ht="15"/>
-    <row r="2" spans="5:5" ht="15"/>
-    <row r="3" spans="5:5" ht="15"/>
-    <row r="4" spans="5:5" ht="15"/>
-    <row r="5" spans="5:5" ht="15"/>
-    <row r="6" spans="5:5" ht="15"/>
     <row r="7" spans="5:5" ht="15.75">
       <c r="E7" s="2" t="s">
         <v>100</v>

</xml_diff>